<commit_message>
Additions and bug fixes
</commit_message>
<xml_diff>
--- a/SIN/playback/HINT/HINT.xlsx
+++ b/SIN/playback/HINT/HINT.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwbishop\Documents\GitHub\MATLAB\SIN\playback\HINT\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="225" windowWidth="19440" windowHeight="11700" activeTab="1"/>
   </bookViews>
@@ -5657,72 +5662,6 @@
     <t>25_09</t>
   </si>
   <si>
-    <t>C:\AST\HINT\List01\01.wav</t>
-  </si>
-  <si>
-    <t>C:\AST\HINT\List01\02.wav</t>
-  </si>
-  <si>
-    <t>C:\AST\HINT\List01\03.wav</t>
-  </si>
-  <si>
-    <t>C:\AST\HINT\List01\04.wav</t>
-  </si>
-  <si>
-    <t>C:\AST\HINT\List01\05.wav</t>
-  </si>
-  <si>
-    <t>C:\AST\HINT\List01\06.wav</t>
-  </si>
-  <si>
-    <t>C:\AST\HINT\List01\07.wav</t>
-  </si>
-  <si>
-    <t>C:\AST\HINT\List01\08.wav</t>
-  </si>
-  <si>
-    <t>C:\AST\HINT\List01\09.wav</t>
-  </si>
-  <si>
-    <t>C:\AST\HINT\List01\10.wav</t>
-  </si>
-  <si>
-    <t>C:\AST\HINT\List02\01.wav</t>
-  </si>
-  <si>
-    <t>C:\AST\HINT\List02\02.wav</t>
-  </si>
-  <si>
-    <t>C:\AST\HINT\List02\03.wav</t>
-  </si>
-  <si>
-    <t>C:\AST\HINT\List02\04.wav</t>
-  </si>
-  <si>
-    <t>C:\AST\HINT\List02\05.wav</t>
-  </si>
-  <si>
-    <t>C:\AST\HINT\List02\06.wav</t>
-  </si>
-  <si>
-    <t>C:\AST\HINT\List02\07.wav</t>
-  </si>
-  <si>
-    <t>C:\AST\HINT\List02\08.wav</t>
-  </si>
-  <si>
-    <t>C:\AST\HINT\List02\09.wav</t>
-  </si>
-  <si>
-    <t>C:\AST\HINT\List02\10.wav</t>
-  </si>
-  <si>
-    <t>C:\AST\HINT\List03\01.wav</t>
-  </si>
-  <si>
-    <t>C:\AST\HINT\List03\02.wav</t>
-  </si>
-  <si>
     <t>C:\AST\HINT\List03\03.wav</t>
   </si>
   <si>
@@ -6332,9 +6271,6 @@
     <t>C:\AST\HINT\List23\05.wav</t>
   </si>
   <si>
-    <t>C:\AST\HINT\List23\06.wav</t>
-  </si>
-  <si>
     <t>C:\AST\HINT\List23\07.wav</t>
   </si>
   <si>
@@ -6405,6 +6341,75 @@
   </si>
   <si>
     <t>C:\AST\HINT\List25\10.wav</t>
+  </si>
+  <si>
+    <t>\List23\06.wav</t>
+  </si>
+  <si>
+    <t>List01\01.wav</t>
+  </si>
+  <si>
+    <t>List01\02.wav</t>
+  </si>
+  <si>
+    <t>List01\03.wav</t>
+  </si>
+  <si>
+    <t>List01\04.wav</t>
+  </si>
+  <si>
+    <t>List01\05.wav</t>
+  </si>
+  <si>
+    <t>List01\06.wav</t>
+  </si>
+  <si>
+    <t>List01\07.wav</t>
+  </si>
+  <si>
+    <t>List01\08.wav</t>
+  </si>
+  <si>
+    <t>List01\09.wav</t>
+  </si>
+  <si>
+    <t>List01\10.wav</t>
+  </si>
+  <si>
+    <t>List02\01.wav</t>
+  </si>
+  <si>
+    <t>List02\02.wav</t>
+  </si>
+  <si>
+    <t>List02\03.wav</t>
+  </si>
+  <si>
+    <t>List02\04.wav</t>
+  </si>
+  <si>
+    <t>List02\05.wav</t>
+  </si>
+  <si>
+    <t>List02\06.wav</t>
+  </si>
+  <si>
+    <t>List02\07.wav</t>
+  </si>
+  <si>
+    <t>List02\08.wav</t>
+  </si>
+  <si>
+    <t>List02\09.wav</t>
+  </si>
+  <si>
+    <t>List02\10.wav</t>
+  </si>
+  <si>
+    <t>List03\01.wav</t>
+  </si>
+  <si>
+    <t>List03\02.wav</t>
   </si>
 </sst>
 </file>
@@ -6460,6 +6465,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -6507,7 +6515,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6542,7 +6550,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6754,7 +6762,7 @@
   <dimension ref="A1:F465"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A274" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A430" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D282" sqref="D282"/>
     </sheetView>
   </sheetViews>
@@ -14215,8 +14223,8 @@
   <dimension ref="A1:D278"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B251"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14246,7 +14254,7 @@
         <v>1646</v>
       </c>
       <c r="B2" t="s">
-        <v>1880</v>
+        <v>2108</v>
       </c>
       <c r="C2" t="s">
         <v>1396</v>
@@ -14260,7 +14268,7 @@
         <v>1647</v>
       </c>
       <c r="B3" t="s">
-        <v>1881</v>
+        <v>2109</v>
       </c>
       <c r="C3" t="s">
         <v>1397</v>
@@ -14274,7 +14282,7 @@
         <v>1648</v>
       </c>
       <c r="B4" t="s">
-        <v>1882</v>
+        <v>2110</v>
       </c>
       <c r="C4" t="s">
         <v>1398</v>
@@ -14288,7 +14296,7 @@
         <v>1649</v>
       </c>
       <c r="B5" t="s">
-        <v>1883</v>
+        <v>2111</v>
       </c>
       <c r="C5" t="s">
         <v>1399</v>
@@ -14302,7 +14310,7 @@
         <v>1650</v>
       </c>
       <c r="B6" t="s">
-        <v>1884</v>
+        <v>2112</v>
       </c>
       <c r="C6" t="s">
         <v>1400</v>
@@ -14316,7 +14324,7 @@
         <v>1651</v>
       </c>
       <c r="B7" t="s">
-        <v>1885</v>
+        <v>2113</v>
       </c>
       <c r="C7" t="s">
         <v>1401</v>
@@ -14330,7 +14338,7 @@
         <v>1652</v>
       </c>
       <c r="B8" t="s">
-        <v>1886</v>
+        <v>2114</v>
       </c>
       <c r="C8" t="s">
         <v>1402</v>
@@ -14344,7 +14352,7 @@
         <v>1653</v>
       </c>
       <c r="B9" t="s">
-        <v>1887</v>
+        <v>2115</v>
       </c>
       <c r="C9" t="s">
         <v>1403</v>
@@ -14358,7 +14366,7 @@
         <v>1654</v>
       </c>
       <c r="B10" t="s">
-        <v>1888</v>
+        <v>2116</v>
       </c>
       <c r="C10" t="s">
         <v>1404</v>
@@ -14372,7 +14380,7 @@
         <v>1655</v>
       </c>
       <c r="B11" t="s">
-        <v>1889</v>
+        <v>2117</v>
       </c>
       <c r="C11" t="s">
         <v>1405</v>
@@ -14386,7 +14394,7 @@
         <v>1656</v>
       </c>
       <c r="B12" t="s">
-        <v>1890</v>
+        <v>2118</v>
       </c>
       <c r="C12" t="s">
         <v>1406</v>
@@ -14400,7 +14408,7 @@
         <v>1657</v>
       </c>
       <c r="B13" t="s">
-        <v>1891</v>
+        <v>2119</v>
       </c>
       <c r="C13" t="s">
         <v>1407</v>
@@ -14414,7 +14422,7 @@
         <v>1658</v>
       </c>
       <c r="B14" t="s">
-        <v>1892</v>
+        <v>2120</v>
       </c>
       <c r="C14" t="s">
         <v>1408</v>
@@ -14428,7 +14436,7 @@
         <v>1659</v>
       </c>
       <c r="B15" t="s">
-        <v>1893</v>
+        <v>2121</v>
       </c>
       <c r="C15" t="s">
         <v>1409</v>
@@ -14442,7 +14450,7 @@
         <v>1660</v>
       </c>
       <c r="B16" t="s">
-        <v>1894</v>
+        <v>2122</v>
       </c>
       <c r="C16" t="s">
         <v>1410</v>
@@ -14456,7 +14464,7 @@
         <v>1661</v>
       </c>
       <c r="B17" t="s">
-        <v>1895</v>
+        <v>2123</v>
       </c>
       <c r="C17" t="s">
         <v>1411</v>
@@ -14470,7 +14478,7 @@
         <v>1662</v>
       </c>
       <c r="B18" t="s">
-        <v>1896</v>
+        <v>2124</v>
       </c>
       <c r="C18" t="s">
         <v>1412</v>
@@ -14484,7 +14492,7 @@
         <v>1663</v>
       </c>
       <c r="B19" t="s">
-        <v>1897</v>
+        <v>2125</v>
       </c>
       <c r="C19" t="s">
         <v>1413</v>
@@ -14498,7 +14506,7 @@
         <v>1664</v>
       </c>
       <c r="B20" t="s">
-        <v>1898</v>
+        <v>2126</v>
       </c>
       <c r="C20" t="s">
         <v>1414</v>
@@ -14512,7 +14520,7 @@
         <v>1665</v>
       </c>
       <c r="B21" t="s">
-        <v>1899</v>
+        <v>2127</v>
       </c>
       <c r="C21" t="s">
         <v>1415</v>
@@ -14526,7 +14534,7 @@
         <v>1666</v>
       </c>
       <c r="B22" t="s">
-        <v>1900</v>
+        <v>2128</v>
       </c>
       <c r="C22" t="s">
         <v>1416</v>
@@ -14540,7 +14548,7 @@
         <v>1667</v>
       </c>
       <c r="B23" t="s">
-        <v>1901</v>
+        <v>2129</v>
       </c>
       <c r="C23" t="s">
         <v>1417</v>
@@ -14554,7 +14562,7 @@
         <v>1668</v>
       </c>
       <c r="B24" t="s">
-        <v>1902</v>
+        <v>1880</v>
       </c>
       <c r="C24" t="s">
         <v>1418</v>
@@ -14568,7 +14576,7 @@
         <v>1669</v>
       </c>
       <c r="B25" t="s">
-        <v>1903</v>
+        <v>1881</v>
       </c>
       <c r="C25" t="s">
         <v>1419</v>
@@ -14582,7 +14590,7 @@
         <v>1670</v>
       </c>
       <c r="B26" t="s">
-        <v>1904</v>
+        <v>1882</v>
       </c>
       <c r="C26" t="s">
         <v>1420</v>
@@ -14596,7 +14604,7 @@
         <v>1671</v>
       </c>
       <c r="B27" t="s">
-        <v>1905</v>
+        <v>1883</v>
       </c>
       <c r="C27" t="s">
         <v>1421</v>
@@ -14610,7 +14618,7 @@
         <v>1672</v>
       </c>
       <c r="B28" t="s">
-        <v>1906</v>
+        <v>1884</v>
       </c>
       <c r="C28" t="s">
         <v>1422</v>
@@ -14624,7 +14632,7 @@
         <v>1673</v>
       </c>
       <c r="B29" t="s">
-        <v>1907</v>
+        <v>1885</v>
       </c>
       <c r="C29" t="s">
         <v>1423</v>
@@ -14638,7 +14646,7 @@
         <v>1674</v>
       </c>
       <c r="B30" t="s">
-        <v>1908</v>
+        <v>1886</v>
       </c>
       <c r="C30" t="s">
         <v>1424</v>
@@ -14652,7 +14660,7 @@
         <v>1675</v>
       </c>
       <c r="B31" t="s">
-        <v>1909</v>
+        <v>1887</v>
       </c>
       <c r="C31" t="s">
         <v>1425</v>
@@ -14666,7 +14674,7 @@
         <v>1676</v>
       </c>
       <c r="B32" t="s">
-        <v>1910</v>
+        <v>1888</v>
       </c>
       <c r="C32" t="s">
         <v>1426</v>
@@ -14680,7 +14688,7 @@
         <v>1677</v>
       </c>
       <c r="B33" t="s">
-        <v>1911</v>
+        <v>1889</v>
       </c>
       <c r="C33" t="s">
         <v>1427</v>
@@ -14694,7 +14702,7 @@
         <v>1678</v>
       </c>
       <c r="B34" t="s">
-        <v>1912</v>
+        <v>1890</v>
       </c>
       <c r="C34" t="s">
         <v>1428</v>
@@ -14708,7 +14716,7 @@
         <v>1679</v>
       </c>
       <c r="B35" t="s">
-        <v>1913</v>
+        <v>1891</v>
       </c>
       <c r="C35" t="s">
         <v>1429</v>
@@ -14722,7 +14730,7 @@
         <v>1680</v>
       </c>
       <c r="B36" t="s">
-        <v>1914</v>
+        <v>1892</v>
       </c>
       <c r="C36" t="s">
         <v>1430</v>
@@ -14736,7 +14744,7 @@
         <v>1681</v>
       </c>
       <c r="B37" t="s">
-        <v>1915</v>
+        <v>1893</v>
       </c>
       <c r="C37" t="s">
         <v>1431</v>
@@ -14750,7 +14758,7 @@
         <v>1682</v>
       </c>
       <c r="B38" t="s">
-        <v>1916</v>
+        <v>1894</v>
       </c>
       <c r="C38" t="s">
         <v>1432</v>
@@ -14764,7 +14772,7 @@
         <v>1683</v>
       </c>
       <c r="B39" t="s">
-        <v>1917</v>
+        <v>1895</v>
       </c>
       <c r="C39" t="s">
         <v>1433</v>
@@ -14778,7 +14786,7 @@
         <v>1684</v>
       </c>
       <c r="B40" t="s">
-        <v>1918</v>
+        <v>1896</v>
       </c>
       <c r="C40" t="s">
         <v>1434</v>
@@ -14792,7 +14800,7 @@
         <v>1685</v>
       </c>
       <c r="B41" t="s">
-        <v>1919</v>
+        <v>1897</v>
       </c>
       <c r="C41" t="s">
         <v>1435</v>
@@ -14806,7 +14814,7 @@
         <v>1686</v>
       </c>
       <c r="B42" t="s">
-        <v>1920</v>
+        <v>1898</v>
       </c>
       <c r="C42" t="s">
         <v>1436</v>
@@ -14820,7 +14828,7 @@
         <v>1687</v>
       </c>
       <c r="B43" t="s">
-        <v>1921</v>
+        <v>1899</v>
       </c>
       <c r="C43" t="s">
         <v>1437</v>
@@ -14834,7 +14842,7 @@
         <v>1688</v>
       </c>
       <c r="B44" t="s">
-        <v>1922</v>
+        <v>1900</v>
       </c>
       <c r="C44" t="s">
         <v>1438</v>
@@ -14848,7 +14856,7 @@
         <v>1689</v>
       </c>
       <c r="B45" t="s">
-        <v>1923</v>
+        <v>1901</v>
       </c>
       <c r="C45" t="s">
         <v>1439</v>
@@ -14862,7 +14870,7 @@
         <v>1690</v>
       </c>
       <c r="B46" t="s">
-        <v>1924</v>
+        <v>1902</v>
       </c>
       <c r="C46" t="s">
         <v>1440</v>
@@ -14876,7 +14884,7 @@
         <v>1691</v>
       </c>
       <c r="B47" t="s">
-        <v>1925</v>
+        <v>1903</v>
       </c>
       <c r="C47" t="s">
         <v>1441</v>
@@ -14890,7 +14898,7 @@
         <v>1692</v>
       </c>
       <c r="B48" t="s">
-        <v>1926</v>
+        <v>1904</v>
       </c>
       <c r="C48" t="s">
         <v>1442</v>
@@ -14904,7 +14912,7 @@
         <v>1693</v>
       </c>
       <c r="B49" t="s">
-        <v>1927</v>
+        <v>1905</v>
       </c>
       <c r="C49" t="s">
         <v>1443</v>
@@ -14918,7 +14926,7 @@
         <v>1694</v>
       </c>
       <c r="B50" t="s">
-        <v>1928</v>
+        <v>1906</v>
       </c>
       <c r="C50" t="s">
         <v>1444</v>
@@ -14932,7 +14940,7 @@
         <v>1695</v>
       </c>
       <c r="B51" t="s">
-        <v>1929</v>
+        <v>1907</v>
       </c>
       <c r="C51" t="s">
         <v>1445</v>
@@ -14946,7 +14954,7 @@
         <v>1696</v>
       </c>
       <c r="B52" t="s">
-        <v>1930</v>
+        <v>1908</v>
       </c>
       <c r="C52" t="s">
         <v>1446</v>
@@ -14960,7 +14968,7 @@
         <v>1697</v>
       </c>
       <c r="B53" t="s">
-        <v>1931</v>
+        <v>1909</v>
       </c>
       <c r="C53" t="s">
         <v>1447</v>
@@ -14974,7 +14982,7 @@
         <v>1698</v>
       </c>
       <c r="B54" t="s">
-        <v>1932</v>
+        <v>1910</v>
       </c>
       <c r="C54" t="s">
         <v>1448</v>
@@ -14988,7 +14996,7 @@
         <v>1699</v>
       </c>
       <c r="B55" t="s">
-        <v>1933</v>
+        <v>1911</v>
       </c>
       <c r="C55" t="s">
         <v>1449</v>
@@ -15002,7 +15010,7 @@
         <v>1700</v>
       </c>
       <c r="B56" t="s">
-        <v>1934</v>
+        <v>1912</v>
       </c>
       <c r="C56" t="s">
         <v>1450</v>
@@ -15016,7 +15024,7 @@
         <v>1701</v>
       </c>
       <c r="B57" t="s">
-        <v>1935</v>
+        <v>1913</v>
       </c>
       <c r="C57" t="s">
         <v>1451</v>
@@ -15030,7 +15038,7 @@
         <v>1702</v>
       </c>
       <c r="B58" t="s">
-        <v>1936</v>
+        <v>1914</v>
       </c>
       <c r="C58" t="s">
         <v>1452</v>
@@ -15044,7 +15052,7 @@
         <v>1703</v>
       </c>
       <c r="B59" t="s">
-        <v>1937</v>
+        <v>1915</v>
       </c>
       <c r="C59" t="s">
         <v>1453</v>
@@ -15058,7 +15066,7 @@
         <v>1704</v>
       </c>
       <c r="B60" t="s">
-        <v>1938</v>
+        <v>1916</v>
       </c>
       <c r="C60" t="s">
         <v>1454</v>
@@ -15072,7 +15080,7 @@
         <v>1705</v>
       </c>
       <c r="B61" t="s">
-        <v>1939</v>
+        <v>1917</v>
       </c>
       <c r="C61" t="s">
         <v>1455</v>
@@ -15086,7 +15094,7 @@
         <v>1706</v>
       </c>
       <c r="B62" t="s">
-        <v>1940</v>
+        <v>1918</v>
       </c>
       <c r="C62" t="s">
         <v>1456</v>
@@ -15100,7 +15108,7 @@
         <v>1707</v>
       </c>
       <c r="B63" t="s">
-        <v>1941</v>
+        <v>1919</v>
       </c>
       <c r="C63" t="s">
         <v>1457</v>
@@ -15114,7 +15122,7 @@
         <v>1708</v>
       </c>
       <c r="B64" t="s">
-        <v>1942</v>
+        <v>1920</v>
       </c>
       <c r="C64" t="s">
         <v>1458</v>
@@ -15128,7 +15136,7 @@
         <v>1709</v>
       </c>
       <c r="B65" t="s">
-        <v>1943</v>
+        <v>1921</v>
       </c>
       <c r="C65" t="s">
         <v>1459</v>
@@ -15142,7 +15150,7 @@
         <v>1710</v>
       </c>
       <c r="B66" t="s">
-        <v>1944</v>
+        <v>1922</v>
       </c>
       <c r="C66" t="s">
         <v>1460</v>
@@ -15156,7 +15164,7 @@
         <v>1711</v>
       </c>
       <c r="B67" t="s">
-        <v>1945</v>
+        <v>1923</v>
       </c>
       <c r="C67" t="s">
         <v>1461</v>
@@ -15170,7 +15178,7 @@
         <v>1712</v>
       </c>
       <c r="B68" t="s">
-        <v>1946</v>
+        <v>1924</v>
       </c>
       <c r="C68" t="s">
         <v>1462</v>
@@ -15184,7 +15192,7 @@
         <v>1713</v>
       </c>
       <c r="B69" t="s">
-        <v>1947</v>
+        <v>1925</v>
       </c>
       <c r="C69" t="s">
         <v>1463</v>
@@ -15198,7 +15206,7 @@
         <v>1714</v>
       </c>
       <c r="B70" t="s">
-        <v>1948</v>
+        <v>1926</v>
       </c>
       <c r="C70" t="s">
         <v>1464</v>
@@ -15212,7 +15220,7 @@
         <v>1715</v>
       </c>
       <c r="B71" t="s">
-        <v>1949</v>
+        <v>1927</v>
       </c>
       <c r="C71" t="s">
         <v>1465</v>
@@ -15226,7 +15234,7 @@
         <v>1716</v>
       </c>
       <c r="B72" t="s">
-        <v>1950</v>
+        <v>1928</v>
       </c>
       <c r="C72" t="s">
         <v>1466</v>
@@ -15240,7 +15248,7 @@
         <v>1717</v>
       </c>
       <c r="B73" t="s">
-        <v>1951</v>
+        <v>1929</v>
       </c>
       <c r="C73" t="s">
         <v>1467</v>
@@ -15254,7 +15262,7 @@
         <v>1718</v>
       </c>
       <c r="B74" t="s">
-        <v>1952</v>
+        <v>1930</v>
       </c>
       <c r="C74" t="s">
         <v>1468</v>
@@ -15268,7 +15276,7 @@
         <v>1719</v>
       </c>
       <c r="B75" t="s">
-        <v>1953</v>
+        <v>1931</v>
       </c>
       <c r="C75" t="s">
         <v>1469</v>
@@ -15282,7 +15290,7 @@
         <v>1720</v>
       </c>
       <c r="B76" t="s">
-        <v>1954</v>
+        <v>1932</v>
       </c>
       <c r="C76" t="s">
         <v>1470</v>
@@ -15296,7 +15304,7 @@
         <v>1721</v>
       </c>
       <c r="B77" t="s">
-        <v>1955</v>
+        <v>1933</v>
       </c>
       <c r="C77" t="s">
         <v>1471</v>
@@ -15310,7 +15318,7 @@
         <v>1722</v>
       </c>
       <c r="B78" t="s">
-        <v>1956</v>
+        <v>1934</v>
       </c>
       <c r="C78" t="s">
         <v>1472</v>
@@ -15324,7 +15332,7 @@
         <v>1723</v>
       </c>
       <c r="B79" t="s">
-        <v>1957</v>
+        <v>1935</v>
       </c>
       <c r="C79" t="s">
         <v>1473</v>
@@ -15338,7 +15346,7 @@
         <v>1724</v>
       </c>
       <c r="B80" t="s">
-        <v>1958</v>
+        <v>1936</v>
       </c>
       <c r="C80" t="s">
         <v>1474</v>
@@ -15352,7 +15360,7 @@
         <v>1725</v>
       </c>
       <c r="B81" t="s">
-        <v>1959</v>
+        <v>1937</v>
       </c>
       <c r="C81" t="s">
         <v>1475</v>
@@ -15366,7 +15374,7 @@
         <v>1726</v>
       </c>
       <c r="B82" t="s">
-        <v>1960</v>
+        <v>1938</v>
       </c>
       <c r="C82" t="s">
         <v>1476</v>
@@ -15380,7 +15388,7 @@
         <v>1727</v>
       </c>
       <c r="B83" t="s">
-        <v>1961</v>
+        <v>1939</v>
       </c>
       <c r="C83" t="s">
         <v>1477</v>
@@ -15394,7 +15402,7 @@
         <v>1728</v>
       </c>
       <c r="B84" t="s">
-        <v>1962</v>
+        <v>1940</v>
       </c>
       <c r="C84" t="s">
         <v>1478</v>
@@ -15408,7 +15416,7 @@
         <v>1729</v>
       </c>
       <c r="B85" t="s">
-        <v>1963</v>
+        <v>1941</v>
       </c>
       <c r="C85" t="s">
         <v>1479</v>
@@ -15422,7 +15430,7 @@
         <v>1730</v>
       </c>
       <c r="B86" t="s">
-        <v>1964</v>
+        <v>1942</v>
       </c>
       <c r="C86" t="s">
         <v>1480</v>
@@ -15436,7 +15444,7 @@
         <v>1731</v>
       </c>
       <c r="B87" t="s">
-        <v>1965</v>
+        <v>1943</v>
       </c>
       <c r="C87" t="s">
         <v>1481</v>
@@ -15450,7 +15458,7 @@
         <v>1732</v>
       </c>
       <c r="B88" t="s">
-        <v>1966</v>
+        <v>1944</v>
       </c>
       <c r="C88" t="s">
         <v>1482</v>
@@ -15464,7 +15472,7 @@
         <v>1733</v>
       </c>
       <c r="B89" t="s">
-        <v>1967</v>
+        <v>1945</v>
       </c>
       <c r="C89" t="s">
         <v>1483</v>
@@ -15478,7 +15486,7 @@
         <v>1734</v>
       </c>
       <c r="B90" t="s">
-        <v>1968</v>
+        <v>1946</v>
       </c>
       <c r="C90" t="s">
         <v>1484</v>
@@ -15492,7 +15500,7 @@
         <v>1735</v>
       </c>
       <c r="B91" t="s">
-        <v>1969</v>
+        <v>1947</v>
       </c>
       <c r="C91" t="s">
         <v>1485</v>
@@ -15506,7 +15514,7 @@
         <v>1736</v>
       </c>
       <c r="B92" t="s">
-        <v>1970</v>
+        <v>1948</v>
       </c>
       <c r="C92" t="s">
         <v>1486</v>
@@ -15520,7 +15528,7 @@
         <v>1737</v>
       </c>
       <c r="B93" t="s">
-        <v>1971</v>
+        <v>1949</v>
       </c>
       <c r="C93" t="s">
         <v>1487</v>
@@ -15534,7 +15542,7 @@
         <v>1738</v>
       </c>
       <c r="B94" t="s">
-        <v>1972</v>
+        <v>1950</v>
       </c>
       <c r="C94" t="s">
         <v>1488</v>
@@ -15548,7 +15556,7 @@
         <v>1739</v>
       </c>
       <c r="B95" t="s">
-        <v>1973</v>
+        <v>1951</v>
       </c>
       <c r="C95" t="s">
         <v>1489</v>
@@ -15562,7 +15570,7 @@
         <v>1740</v>
       </c>
       <c r="B96" t="s">
-        <v>1974</v>
+        <v>1952</v>
       </c>
       <c r="C96" t="s">
         <v>1490</v>
@@ -15576,7 +15584,7 @@
         <v>1741</v>
       </c>
       <c r="B97" t="s">
-        <v>1975</v>
+        <v>1953</v>
       </c>
       <c r="C97" t="s">
         <v>1491</v>
@@ -15590,7 +15598,7 @@
         <v>1742</v>
       </c>
       <c r="B98" t="s">
-        <v>1976</v>
+        <v>1954</v>
       </c>
       <c r="C98" t="s">
         <v>1492</v>
@@ -15604,7 +15612,7 @@
         <v>1743</v>
       </c>
       <c r="B99" t="s">
-        <v>1977</v>
+        <v>1955</v>
       </c>
       <c r="C99" t="s">
         <v>1493</v>
@@ -15618,7 +15626,7 @@
         <v>1744</v>
       </c>
       <c r="B100" t="s">
-        <v>1978</v>
+        <v>1956</v>
       </c>
       <c r="C100" t="s">
         <v>1494</v>
@@ -15632,7 +15640,7 @@
         <v>61</v>
       </c>
       <c r="B101" t="s">
-        <v>1979</v>
+        <v>1957</v>
       </c>
       <c r="C101" t="s">
         <v>1495</v>
@@ -15646,7 +15654,7 @@
         <v>1745</v>
       </c>
       <c r="B102" t="s">
-        <v>1980</v>
+        <v>1958</v>
       </c>
       <c r="C102" t="s">
         <v>1496</v>
@@ -15660,7 +15668,7 @@
         <v>1746</v>
       </c>
       <c r="B103" t="s">
-        <v>1981</v>
+        <v>1959</v>
       </c>
       <c r="C103" t="s">
         <v>1497</v>
@@ -15674,7 +15682,7 @@
         <v>1747</v>
       </c>
       <c r="B104" t="s">
-        <v>1982</v>
+        <v>1960</v>
       </c>
       <c r="C104" t="s">
         <v>1498</v>
@@ -15688,7 +15696,7 @@
         <v>1748</v>
       </c>
       <c r="B105" t="s">
-        <v>1983</v>
+        <v>1961</v>
       </c>
       <c r="C105" t="s">
         <v>1499</v>
@@ -15702,7 +15710,7 @@
         <v>1749</v>
       </c>
       <c r="B106" t="s">
-        <v>1984</v>
+        <v>1962</v>
       </c>
       <c r="C106" t="s">
         <v>1500</v>
@@ -15716,7 +15724,7 @@
         <v>1750</v>
       </c>
       <c r="B107" t="s">
-        <v>1985</v>
+        <v>1963</v>
       </c>
       <c r="C107" t="s">
         <v>1501</v>
@@ -15730,7 +15738,7 @@
         <v>1751</v>
       </c>
       <c r="B108" t="s">
-        <v>1986</v>
+        <v>1964</v>
       </c>
       <c r="C108" t="s">
         <v>1502</v>
@@ -15744,7 +15752,7 @@
         <v>1752</v>
       </c>
       <c r="B109" t="s">
-        <v>1987</v>
+        <v>1965</v>
       </c>
       <c r="C109" t="s">
         <v>1503</v>
@@ -15758,7 +15766,7 @@
         <v>1753</v>
       </c>
       <c r="B110" t="s">
-        <v>1988</v>
+        <v>1966</v>
       </c>
       <c r="C110" t="s">
         <v>1504</v>
@@ -15772,7 +15780,7 @@
         <v>77</v>
       </c>
       <c r="B111" t="s">
-        <v>1989</v>
+        <v>1967</v>
       </c>
       <c r="C111" t="s">
         <v>1505</v>
@@ -15786,7 +15794,7 @@
         <v>1754</v>
       </c>
       <c r="B112" t="s">
-        <v>1990</v>
+        <v>1968</v>
       </c>
       <c r="C112" t="s">
         <v>1506</v>
@@ -15800,7 +15808,7 @@
         <v>1755</v>
       </c>
       <c r="B113" t="s">
-        <v>1991</v>
+        <v>1969</v>
       </c>
       <c r="C113" t="s">
         <v>1507</v>
@@ -15814,7 +15822,7 @@
         <v>1756</v>
       </c>
       <c r="B114" t="s">
-        <v>1992</v>
+        <v>1970</v>
       </c>
       <c r="C114" t="s">
         <v>1508</v>
@@ -15828,7 +15836,7 @@
         <v>1757</v>
       </c>
       <c r="B115" t="s">
-        <v>1993</v>
+        <v>1971</v>
       </c>
       <c r="C115" t="s">
         <v>1509</v>
@@ -15842,7 +15850,7 @@
         <v>1758</v>
       </c>
       <c r="B116" t="s">
-        <v>1994</v>
+        <v>1972</v>
       </c>
       <c r="C116" t="s">
         <v>1510</v>
@@ -15856,7 +15864,7 @@
         <v>1759</v>
       </c>
       <c r="B117" t="s">
-        <v>1995</v>
+        <v>1973</v>
       </c>
       <c r="C117" t="s">
         <v>1511</v>
@@ -15870,7 +15878,7 @@
         <v>1760</v>
       </c>
       <c r="B118" t="s">
-        <v>1996</v>
+        <v>1974</v>
       </c>
       <c r="C118" t="s">
         <v>1512</v>
@@ -15884,7 +15892,7 @@
         <v>1761</v>
       </c>
       <c r="B119" t="s">
-        <v>1997</v>
+        <v>1975</v>
       </c>
       <c r="C119" t="s">
         <v>1513</v>
@@ -15898,7 +15906,7 @@
         <v>1762</v>
       </c>
       <c r="B120" t="s">
-        <v>1998</v>
+        <v>1976</v>
       </c>
       <c r="C120" t="s">
         <v>1514</v>
@@ -15912,7 +15920,7 @@
         <v>93</v>
       </c>
       <c r="B121" t="s">
-        <v>1999</v>
+        <v>1977</v>
       </c>
       <c r="C121" t="s">
         <v>1515</v>
@@ -15926,7 +15934,7 @@
         <v>1763</v>
       </c>
       <c r="B122" t="s">
-        <v>2000</v>
+        <v>1978</v>
       </c>
       <c r="C122" t="s">
         <v>1516</v>
@@ -15940,7 +15948,7 @@
         <v>1764</v>
       </c>
       <c r="B123" t="s">
-        <v>2001</v>
+        <v>1979</v>
       </c>
       <c r="C123" t="s">
         <v>1517</v>
@@ -15954,7 +15962,7 @@
         <v>1765</v>
       </c>
       <c r="B124" t="s">
-        <v>2002</v>
+        <v>1980</v>
       </c>
       <c r="C124" t="s">
         <v>1518</v>
@@ -15968,7 +15976,7 @@
         <v>1766</v>
       </c>
       <c r="B125" t="s">
-        <v>2003</v>
+        <v>1981</v>
       </c>
       <c r="C125" t="s">
         <v>1519</v>
@@ -15982,7 +15990,7 @@
         <v>1767</v>
       </c>
       <c r="B126" t="s">
-        <v>2004</v>
+        <v>1982</v>
       </c>
       <c r="C126" t="s">
         <v>1520</v>
@@ -15996,7 +16004,7 @@
         <v>1768</v>
       </c>
       <c r="B127" t="s">
-        <v>2005</v>
+        <v>1983</v>
       </c>
       <c r="C127" t="s">
         <v>1521</v>
@@ -16010,7 +16018,7 @@
         <v>1769</v>
       </c>
       <c r="B128" t="s">
-        <v>2006</v>
+        <v>1984</v>
       </c>
       <c r="C128" t="s">
         <v>1522</v>
@@ -16024,7 +16032,7 @@
         <v>1770</v>
       </c>
       <c r="B129" t="s">
-        <v>2007</v>
+        <v>1985</v>
       </c>
       <c r="C129" t="s">
         <v>1523</v>
@@ -16038,7 +16046,7 @@
         <v>1771</v>
       </c>
       <c r="B130" t="s">
-        <v>2008</v>
+        <v>1986</v>
       </c>
       <c r="C130" t="s">
         <v>1524</v>
@@ -16052,7 +16060,7 @@
         <v>109</v>
       </c>
       <c r="B131" t="s">
-        <v>2009</v>
+        <v>1987</v>
       </c>
       <c r="C131" t="s">
         <v>1525</v>
@@ -16066,7 +16074,7 @@
         <v>1772</v>
       </c>
       <c r="B132" t="s">
-        <v>2010</v>
+        <v>1988</v>
       </c>
       <c r="C132" t="s">
         <v>1526</v>
@@ -16080,7 +16088,7 @@
         <v>1773</v>
       </c>
       <c r="B133" t="s">
-        <v>2011</v>
+        <v>1989</v>
       </c>
       <c r="C133" t="s">
         <v>1527</v>
@@ -16094,7 +16102,7 @@
         <v>1774</v>
       </c>
       <c r="B134" t="s">
-        <v>2012</v>
+        <v>1990</v>
       </c>
       <c r="C134" t="s">
         <v>1528</v>
@@ -16108,7 +16116,7 @@
         <v>1775</v>
       </c>
       <c r="B135" t="s">
-        <v>2013</v>
+        <v>1991</v>
       </c>
       <c r="C135" t="s">
         <v>1529</v>
@@ -16122,7 +16130,7 @@
         <v>1776</v>
       </c>
       <c r="B136" t="s">
-        <v>2014</v>
+        <v>1992</v>
       </c>
       <c r="C136" t="s">
         <v>1530</v>
@@ -16136,7 +16144,7 @@
         <v>1777</v>
       </c>
       <c r="B137" t="s">
-        <v>2015</v>
+        <v>1993</v>
       </c>
       <c r="C137" t="s">
         <v>1531</v>
@@ -16150,7 +16158,7 @@
         <v>1778</v>
       </c>
       <c r="B138" t="s">
-        <v>2016</v>
+        <v>1994</v>
       </c>
       <c r="C138" t="s">
         <v>1532</v>
@@ -16164,7 +16172,7 @@
         <v>1779</v>
       </c>
       <c r="B139" t="s">
-        <v>2017</v>
+        <v>1995</v>
       </c>
       <c r="C139" t="s">
         <v>1533</v>
@@ -16178,7 +16186,7 @@
         <v>1780</v>
       </c>
       <c r="B140" t="s">
-        <v>2018</v>
+        <v>1996</v>
       </c>
       <c r="C140" t="s">
         <v>1534</v>
@@ -16192,7 +16200,7 @@
         <v>125</v>
       </c>
       <c r="B141" t="s">
-        <v>2019</v>
+        <v>1997</v>
       </c>
       <c r="C141" t="s">
         <v>1535</v>
@@ -16206,7 +16214,7 @@
         <v>1781</v>
       </c>
       <c r="B142" t="s">
-        <v>2020</v>
+        <v>1998</v>
       </c>
       <c r="C142" t="s">
         <v>1536</v>
@@ -16220,7 +16228,7 @@
         <v>1782</v>
       </c>
       <c r="B143" t="s">
-        <v>2021</v>
+        <v>1999</v>
       </c>
       <c r="C143" t="s">
         <v>1537</v>
@@ -16234,7 +16242,7 @@
         <v>1783</v>
       </c>
       <c r="B144" t="s">
-        <v>2022</v>
+        <v>2000</v>
       </c>
       <c r="C144" t="s">
         <v>1538</v>
@@ -16248,7 +16256,7 @@
         <v>1784</v>
       </c>
       <c r="B145" t="s">
-        <v>2023</v>
+        <v>2001</v>
       </c>
       <c r="C145" t="s">
         <v>1539</v>
@@ -16262,7 +16270,7 @@
         <v>1785</v>
       </c>
       <c r="B146" t="s">
-        <v>2024</v>
+        <v>2002</v>
       </c>
       <c r="C146" t="s">
         <v>1540</v>
@@ -16276,7 +16284,7 @@
         <v>1786</v>
       </c>
       <c r="B147" t="s">
-        <v>2025</v>
+        <v>2003</v>
       </c>
       <c r="C147" t="s">
         <v>1541</v>
@@ -16290,7 +16298,7 @@
         <v>1787</v>
       </c>
       <c r="B148" t="s">
-        <v>2026</v>
+        <v>2004</v>
       </c>
       <c r="C148" t="s">
         <v>1542</v>
@@ -16304,7 +16312,7 @@
         <v>1788</v>
       </c>
       <c r="B149" t="s">
-        <v>2027</v>
+        <v>2005</v>
       </c>
       <c r="C149" t="s">
         <v>1543</v>
@@ -16318,7 +16326,7 @@
         <v>1789</v>
       </c>
       <c r="B150" t="s">
-        <v>2028</v>
+        <v>2006</v>
       </c>
       <c r="C150" t="s">
         <v>1544</v>
@@ -16332,7 +16340,7 @@
         <v>141</v>
       </c>
       <c r="B151" t="s">
-        <v>2029</v>
+        <v>2007</v>
       </c>
       <c r="C151" t="s">
         <v>1545</v>
@@ -16346,7 +16354,7 @@
         <v>1790</v>
       </c>
       <c r="B152" t="s">
-        <v>2030</v>
+        <v>2008</v>
       </c>
       <c r="C152" t="s">
         <v>1546</v>
@@ -16360,7 +16368,7 @@
         <v>1791</v>
       </c>
       <c r="B153" t="s">
-        <v>2031</v>
+        <v>2009</v>
       </c>
       <c r="C153" t="s">
         <v>1547</v>
@@ -16374,7 +16382,7 @@
         <v>1792</v>
       </c>
       <c r="B154" t="s">
-        <v>2032</v>
+        <v>2010</v>
       </c>
       <c r="C154" t="s">
         <v>1548</v>
@@ -16388,7 +16396,7 @@
         <v>1793</v>
       </c>
       <c r="B155" t="s">
-        <v>2033</v>
+        <v>2011</v>
       </c>
       <c r="C155" t="s">
         <v>1549</v>
@@ -16402,7 +16410,7 @@
         <v>1794</v>
       </c>
       <c r="B156" t="s">
-        <v>2034</v>
+        <v>2012</v>
       </c>
       <c r="C156" t="s">
         <v>1550</v>
@@ -16416,7 +16424,7 @@
         <v>1795</v>
       </c>
       <c r="B157" t="s">
-        <v>2035</v>
+        <v>2013</v>
       </c>
       <c r="C157" t="s">
         <v>1551</v>
@@ -16430,7 +16438,7 @@
         <v>1796</v>
       </c>
       <c r="B158" t="s">
-        <v>2036</v>
+        <v>2014</v>
       </c>
       <c r="C158" t="s">
         <v>1552</v>
@@ -16444,7 +16452,7 @@
         <v>1797</v>
       </c>
       <c r="B159" t="s">
-        <v>2037</v>
+        <v>2015</v>
       </c>
       <c r="C159" t="s">
         <v>1553</v>
@@ -16458,7 +16466,7 @@
         <v>1798</v>
       </c>
       <c r="B160" t="s">
-        <v>2038</v>
+        <v>2016</v>
       </c>
       <c r="C160" t="s">
         <v>1554</v>
@@ -16472,7 +16480,7 @@
         <v>157</v>
       </c>
       <c r="B161" t="s">
-        <v>2039</v>
+        <v>2017</v>
       </c>
       <c r="C161" t="s">
         <v>1555</v>
@@ -16486,7 +16494,7 @@
         <v>1799</v>
       </c>
       <c r="B162" t="s">
-        <v>2040</v>
+        <v>2018</v>
       </c>
       <c r="C162" t="s">
         <v>1556</v>
@@ -16500,7 +16508,7 @@
         <v>1800</v>
       </c>
       <c r="B163" t="s">
-        <v>2041</v>
+        <v>2019</v>
       </c>
       <c r="C163" t="s">
         <v>1557</v>
@@ -16514,7 +16522,7 @@
         <v>1801</v>
       </c>
       <c r="B164" t="s">
-        <v>2042</v>
+        <v>2020</v>
       </c>
       <c r="C164" t="s">
         <v>1558</v>
@@ -16528,7 +16536,7 @@
         <v>1802</v>
       </c>
       <c r="B165" t="s">
-        <v>2043</v>
+        <v>2021</v>
       </c>
       <c r="C165" t="s">
         <v>1559</v>
@@ -16542,7 +16550,7 @@
         <v>1803</v>
       </c>
       <c r="B166" t="s">
-        <v>2044</v>
+        <v>2022</v>
       </c>
       <c r="C166" t="s">
         <v>1560</v>
@@ -16556,7 +16564,7 @@
         <v>1804</v>
       </c>
       <c r="B167" t="s">
-        <v>2045</v>
+        <v>2023</v>
       </c>
       <c r="C167" t="s">
         <v>1561</v>
@@ -16570,7 +16578,7 @@
         <v>1805</v>
       </c>
       <c r="B168" t="s">
-        <v>2046</v>
+        <v>2024</v>
       </c>
       <c r="C168" t="s">
         <v>1562</v>
@@ -16584,7 +16592,7 @@
         <v>1806</v>
       </c>
       <c r="B169" t="s">
-        <v>2047</v>
+        <v>2025</v>
       </c>
       <c r="C169" t="s">
         <v>1563</v>
@@ -16598,7 +16606,7 @@
         <v>1807</v>
       </c>
       <c r="B170" t="s">
-        <v>2048</v>
+        <v>2026</v>
       </c>
       <c r="C170" t="s">
         <v>1564</v>
@@ -16612,7 +16620,7 @@
         <v>173</v>
       </c>
       <c r="B171" t="s">
-        <v>2049</v>
+        <v>2027</v>
       </c>
       <c r="C171" t="s">
         <v>1565</v>
@@ -16626,7 +16634,7 @@
         <v>1808</v>
       </c>
       <c r="B172" t="s">
-        <v>2050</v>
+        <v>2028</v>
       </c>
       <c r="C172" t="s">
         <v>1566</v>
@@ -16640,7 +16648,7 @@
         <v>1809</v>
       </c>
       <c r="B173" t="s">
-        <v>2051</v>
+        <v>2029</v>
       </c>
       <c r="C173" t="s">
         <v>1567</v>
@@ -16654,7 +16662,7 @@
         <v>1810</v>
       </c>
       <c r="B174" t="s">
-        <v>2052</v>
+        <v>2030</v>
       </c>
       <c r="C174" t="s">
         <v>1568</v>
@@ -16668,7 +16676,7 @@
         <v>1811</v>
       </c>
       <c r="B175" t="s">
-        <v>2053</v>
+        <v>2031</v>
       </c>
       <c r="C175" t="s">
         <v>1569</v>
@@ -16682,7 +16690,7 @@
         <v>1812</v>
       </c>
       <c r="B176" t="s">
-        <v>2054</v>
+        <v>2032</v>
       </c>
       <c r="C176" t="s">
         <v>1570</v>
@@ -16696,7 +16704,7 @@
         <v>1813</v>
       </c>
       <c r="B177" t="s">
-        <v>2055</v>
+        <v>2033</v>
       </c>
       <c r="C177" t="s">
         <v>1571</v>
@@ -16710,7 +16718,7 @@
         <v>1814</v>
       </c>
       <c r="B178" t="s">
-        <v>2056</v>
+        <v>2034</v>
       </c>
       <c r="C178" t="s">
         <v>1572</v>
@@ -16724,7 +16732,7 @@
         <v>1815</v>
       </c>
       <c r="B179" t="s">
-        <v>2057</v>
+        <v>2035</v>
       </c>
       <c r="C179" t="s">
         <v>1573</v>
@@ -16738,7 +16746,7 @@
         <v>1816</v>
       </c>
       <c r="B180" t="s">
-        <v>2058</v>
+        <v>2036</v>
       </c>
       <c r="C180" t="s">
         <v>1574</v>
@@ -16752,7 +16760,7 @@
         <v>189</v>
       </c>
       <c r="B181" t="s">
-        <v>2059</v>
+        <v>2037</v>
       </c>
       <c r="C181" t="s">
         <v>1575</v>
@@ -16766,7 +16774,7 @@
         <v>1817</v>
       </c>
       <c r="B182" t="s">
-        <v>2060</v>
+        <v>2038</v>
       </c>
       <c r="C182" t="s">
         <v>1576</v>
@@ -16780,7 +16788,7 @@
         <v>1818</v>
       </c>
       <c r="B183" t="s">
-        <v>2061</v>
+        <v>2039</v>
       </c>
       <c r="C183" t="s">
         <v>1577</v>
@@ -16794,7 +16802,7 @@
         <v>1819</v>
       </c>
       <c r="B184" t="s">
-        <v>2062</v>
+        <v>2040</v>
       </c>
       <c r="C184" t="s">
         <v>1578</v>
@@ -16808,7 +16816,7 @@
         <v>1820</v>
       </c>
       <c r="B185" t="s">
-        <v>2063</v>
+        <v>2041</v>
       </c>
       <c r="C185" t="s">
         <v>1579</v>
@@ -16822,7 +16830,7 @@
         <v>1821</v>
       </c>
       <c r="B186" t="s">
-        <v>2064</v>
+        <v>2042</v>
       </c>
       <c r="C186" t="s">
         <v>1580</v>
@@ -16836,7 +16844,7 @@
         <v>1822</v>
       </c>
       <c r="B187" t="s">
-        <v>2065</v>
+        <v>2043</v>
       </c>
       <c r="C187" t="s">
         <v>1581</v>
@@ -16850,7 +16858,7 @@
         <v>1823</v>
       </c>
       <c r="B188" t="s">
-        <v>2066</v>
+        <v>2044</v>
       </c>
       <c r="C188" t="s">
         <v>1582</v>
@@ -16864,7 +16872,7 @@
         <v>1824</v>
       </c>
       <c r="B189" t="s">
-        <v>2067</v>
+        <v>2045</v>
       </c>
       <c r="C189" t="s">
         <v>1583</v>
@@ -16878,7 +16886,7 @@
         <v>1825</v>
       </c>
       <c r="B190" t="s">
-        <v>2068</v>
+        <v>2046</v>
       </c>
       <c r="C190" t="s">
         <v>1584</v>
@@ -16892,7 +16900,7 @@
         <v>205</v>
       </c>
       <c r="B191" t="s">
-        <v>2069</v>
+        <v>2047</v>
       </c>
       <c r="C191" t="s">
         <v>1585</v>
@@ -16906,7 +16914,7 @@
         <v>1826</v>
       </c>
       <c r="B192" t="s">
-        <v>2070</v>
+        <v>2048</v>
       </c>
       <c r="C192" t="s">
         <v>1586</v>
@@ -16920,7 +16928,7 @@
         <v>1827</v>
       </c>
       <c r="B193" t="s">
-        <v>2071</v>
+        <v>2049</v>
       </c>
       <c r="C193" t="s">
         <v>1587</v>
@@ -16934,7 +16942,7 @@
         <v>1828</v>
       </c>
       <c r="B194" t="s">
-        <v>2072</v>
+        <v>2050</v>
       </c>
       <c r="C194" t="s">
         <v>1588</v>
@@ -16948,7 +16956,7 @@
         <v>1829</v>
       </c>
       <c r="B195" t="s">
-        <v>2073</v>
+        <v>2051</v>
       </c>
       <c r="C195" t="s">
         <v>1589</v>
@@ -16962,7 +16970,7 @@
         <v>1830</v>
       </c>
       <c r="B196" t="s">
-        <v>2074</v>
+        <v>2052</v>
       </c>
       <c r="C196" t="s">
         <v>1590</v>
@@ -16976,7 +16984,7 @@
         <v>1831</v>
       </c>
       <c r="B197" t="s">
-        <v>2075</v>
+        <v>2053</v>
       </c>
       <c r="C197" t="s">
         <v>1591</v>
@@ -16990,7 +16998,7 @@
         <v>1832</v>
       </c>
       <c r="B198" t="s">
-        <v>2076</v>
+        <v>2054</v>
       </c>
       <c r="C198" t="s">
         <v>1592</v>
@@ -17004,7 +17012,7 @@
         <v>1833</v>
       </c>
       <c r="B199" t="s">
-        <v>2077</v>
+        <v>2055</v>
       </c>
       <c r="C199" t="s">
         <v>1593</v>
@@ -17018,7 +17026,7 @@
         <v>1834</v>
       </c>
       <c r="B200" t="s">
-        <v>2078</v>
+        <v>2056</v>
       </c>
       <c r="C200" t="s">
         <v>1594</v>
@@ -17032,7 +17040,7 @@
         <v>221</v>
       </c>
       <c r="B201" t="s">
-        <v>2079</v>
+        <v>2057</v>
       </c>
       <c r="C201" t="s">
         <v>1595</v>
@@ -17046,7 +17054,7 @@
         <v>1835</v>
       </c>
       <c r="B202" t="s">
-        <v>2080</v>
+        <v>2058</v>
       </c>
       <c r="C202" t="s">
         <v>1596</v>
@@ -17060,7 +17068,7 @@
         <v>1836</v>
       </c>
       <c r="B203" t="s">
-        <v>2081</v>
+        <v>2059</v>
       </c>
       <c r="C203" t="s">
         <v>1597</v>
@@ -17074,7 +17082,7 @@
         <v>1837</v>
       </c>
       <c r="B204" t="s">
-        <v>2082</v>
+        <v>2060</v>
       </c>
       <c r="C204" t="s">
         <v>1598</v>
@@ -17088,7 +17096,7 @@
         <v>1838</v>
       </c>
       <c r="B205" t="s">
-        <v>2083</v>
+        <v>2061</v>
       </c>
       <c r="C205" t="s">
         <v>1599</v>
@@ -17102,7 +17110,7 @@
         <v>1839</v>
       </c>
       <c r="B206" t="s">
-        <v>2084</v>
+        <v>2062</v>
       </c>
       <c r="C206" t="s">
         <v>1600</v>
@@ -17116,7 +17124,7 @@
         <v>1840</v>
       </c>
       <c r="B207" t="s">
-        <v>2085</v>
+        <v>2063</v>
       </c>
       <c r="C207" t="s">
         <v>1601</v>
@@ -17130,7 +17138,7 @@
         <v>1841</v>
       </c>
       <c r="B208" t="s">
-        <v>2086</v>
+        <v>2064</v>
       </c>
       <c r="C208" t="s">
         <v>1602</v>
@@ -17144,7 +17152,7 @@
         <v>1842</v>
       </c>
       <c r="B209" t="s">
-        <v>2087</v>
+        <v>2065</v>
       </c>
       <c r="C209" t="s">
         <v>1603</v>
@@ -17158,7 +17166,7 @@
         <v>1843</v>
       </c>
       <c r="B210" t="s">
-        <v>2088</v>
+        <v>2066</v>
       </c>
       <c r="C210" t="s">
         <v>1604</v>
@@ -17172,7 +17180,7 @@
         <v>237</v>
       </c>
       <c r="B211" t="s">
-        <v>2089</v>
+        <v>2067</v>
       </c>
       <c r="C211" t="s">
         <v>1605</v>
@@ -17186,7 +17194,7 @@
         <v>1844</v>
       </c>
       <c r="B212" t="s">
-        <v>2090</v>
+        <v>2068</v>
       </c>
       <c r="C212" t="s">
         <v>1606</v>
@@ -17200,7 +17208,7 @@
         <v>1845</v>
       </c>
       <c r="B213" t="s">
-        <v>2091</v>
+        <v>2069</v>
       </c>
       <c r="C213" t="s">
         <v>1607</v>
@@ -17214,7 +17222,7 @@
         <v>1846</v>
       </c>
       <c r="B214" t="s">
-        <v>2092</v>
+        <v>2070</v>
       </c>
       <c r="C214" t="s">
         <v>1608</v>
@@ -17228,7 +17236,7 @@
         <v>1847</v>
       </c>
       <c r="B215" t="s">
-        <v>2093</v>
+        <v>2071</v>
       </c>
       <c r="C215" t="s">
         <v>1609</v>
@@ -17242,7 +17250,7 @@
         <v>1848</v>
       </c>
       <c r="B216" t="s">
-        <v>2094</v>
+        <v>2072</v>
       </c>
       <c r="C216" t="s">
         <v>1610</v>
@@ -17256,7 +17264,7 @@
         <v>1849</v>
       </c>
       <c r="B217" t="s">
-        <v>2095</v>
+        <v>2073</v>
       </c>
       <c r="C217" t="s">
         <v>1611</v>
@@ -17270,7 +17278,7 @@
         <v>1850</v>
       </c>
       <c r="B218" t="s">
-        <v>2096</v>
+        <v>2074</v>
       </c>
       <c r="C218" t="s">
         <v>1612</v>
@@ -17284,7 +17292,7 @@
         <v>1851</v>
       </c>
       <c r="B219" t="s">
-        <v>2097</v>
+        <v>2075</v>
       </c>
       <c r="C219" t="s">
         <v>1613</v>
@@ -17298,7 +17306,7 @@
         <v>1852</v>
       </c>
       <c r="B220" t="s">
-        <v>2098</v>
+        <v>2076</v>
       </c>
       <c r="C220" t="s">
         <v>1614</v>
@@ -17312,7 +17320,7 @@
         <v>253</v>
       </c>
       <c r="B221" t="s">
-        <v>2099</v>
+        <v>2077</v>
       </c>
       <c r="C221" t="s">
         <v>1615</v>
@@ -17326,7 +17334,7 @@
         <v>1853</v>
       </c>
       <c r="B222" t="s">
-        <v>2100</v>
+        <v>2078</v>
       </c>
       <c r="C222" t="s">
         <v>1616</v>
@@ -17340,7 +17348,7 @@
         <v>1854</v>
       </c>
       <c r="B223" t="s">
-        <v>2101</v>
+        <v>2079</v>
       </c>
       <c r="C223" t="s">
         <v>1617</v>
@@ -17354,7 +17362,7 @@
         <v>1855</v>
       </c>
       <c r="B224" t="s">
-        <v>2102</v>
+        <v>2080</v>
       </c>
       <c r="C224" t="s">
         <v>1618</v>
@@ -17368,7 +17376,7 @@
         <v>1856</v>
       </c>
       <c r="B225" t="s">
-        <v>2103</v>
+        <v>2081</v>
       </c>
       <c r="C225" t="s">
         <v>1619</v>
@@ -17382,7 +17390,7 @@
         <v>1857</v>
       </c>
       <c r="B226" t="s">
-        <v>2104</v>
+        <v>2082</v>
       </c>
       <c r="C226" t="s">
         <v>1620</v>
@@ -17396,7 +17404,7 @@
         <v>1858</v>
       </c>
       <c r="B227" t="s">
-        <v>2105</v>
+        <v>2107</v>
       </c>
       <c r="C227" t="s">
         <v>1621</v>
@@ -17410,7 +17418,7 @@
         <v>1859</v>
       </c>
       <c r="B228" t="s">
-        <v>2106</v>
+        <v>2083</v>
       </c>
       <c r="C228" t="s">
         <v>1622</v>
@@ -17424,7 +17432,7 @@
         <v>1860</v>
       </c>
       <c r="B229" t="s">
-        <v>2107</v>
+        <v>2084</v>
       </c>
       <c r="C229" t="s">
         <v>1623</v>
@@ -17438,7 +17446,7 @@
         <v>1861</v>
       </c>
       <c r="B230" t="s">
-        <v>2108</v>
+        <v>2085</v>
       </c>
       <c r="C230" t="s">
         <v>1624</v>
@@ -17452,7 +17460,7 @@
         <v>269</v>
       </c>
       <c r="B231" t="s">
-        <v>2109</v>
+        <v>2086</v>
       </c>
       <c r="C231" t="s">
         <v>1625</v>
@@ -17466,7 +17474,7 @@
         <v>1862</v>
       </c>
       <c r="B232" t="s">
-        <v>2110</v>
+        <v>2087</v>
       </c>
       <c r="C232" t="s">
         <v>1645</v>
@@ -17480,7 +17488,7 @@
         <v>1863</v>
       </c>
       <c r="B233" t="s">
-        <v>2111</v>
+        <v>2088</v>
       </c>
       <c r="C233" t="s">
         <v>1626</v>
@@ -17494,7 +17502,7 @@
         <v>1864</v>
       </c>
       <c r="B234" t="s">
-        <v>2112</v>
+        <v>2089</v>
       </c>
       <c r="C234" t="s">
         <v>1627</v>
@@ -17508,7 +17516,7 @@
         <v>1865</v>
       </c>
       <c r="B235" t="s">
-        <v>2113</v>
+        <v>2090</v>
       </c>
       <c r="C235" t="s">
         <v>1628</v>
@@ -17522,7 +17530,7 @@
         <v>1866</v>
       </c>
       <c r="B236" t="s">
-        <v>2114</v>
+        <v>2091</v>
       </c>
       <c r="C236" t="s">
         <v>1629</v>
@@ -17536,7 +17544,7 @@
         <v>1867</v>
       </c>
       <c r="B237" t="s">
-        <v>2115</v>
+        <v>2092</v>
       </c>
       <c r="C237" t="s">
         <v>1630</v>
@@ -17550,7 +17558,7 @@
         <v>1868</v>
       </c>
       <c r="B238" t="s">
-        <v>2116</v>
+        <v>2093</v>
       </c>
       <c r="C238" t="s">
         <v>1631</v>
@@ -17564,7 +17572,7 @@
         <v>1869</v>
       </c>
       <c r="B239" t="s">
-        <v>2117</v>
+        <v>2094</v>
       </c>
       <c r="C239" t="s">
         <v>1632</v>
@@ -17578,7 +17586,7 @@
         <v>1870</v>
       </c>
       <c r="B240" t="s">
-        <v>2118</v>
+        <v>2095</v>
       </c>
       <c r="C240" t="s">
         <v>1633</v>
@@ -17592,7 +17600,7 @@
         <v>285</v>
       </c>
       <c r="B241" t="s">
-        <v>2119</v>
+        <v>2096</v>
       </c>
       <c r="C241" t="s">
         <v>1634</v>
@@ -17606,7 +17614,7 @@
         <v>1871</v>
       </c>
       <c r="B242" t="s">
-        <v>2120</v>
+        <v>2097</v>
       </c>
       <c r="C242" t="s">
         <v>1635</v>
@@ -17620,7 +17628,7 @@
         <v>1872</v>
       </c>
       <c r="B243" t="s">
-        <v>2121</v>
+        <v>2098</v>
       </c>
       <c r="C243" t="s">
         <v>1636</v>
@@ -17634,7 +17642,7 @@
         <v>1873</v>
       </c>
       <c r="B244" t="s">
-        <v>2122</v>
+        <v>2099</v>
       </c>
       <c r="C244" t="s">
         <v>1637</v>
@@ -17648,7 +17656,7 @@
         <v>1874</v>
       </c>
       <c r="B245" t="s">
-        <v>2123</v>
+        <v>2100</v>
       </c>
       <c r="C245" t="s">
         <v>1638</v>
@@ -17662,7 +17670,7 @@
         <v>1875</v>
       </c>
       <c r="B246" t="s">
-        <v>2124</v>
+        <v>2101</v>
       </c>
       <c r="C246" t="s">
         <v>1639</v>
@@ -17676,7 +17684,7 @@
         <v>1876</v>
       </c>
       <c r="B247" t="s">
-        <v>2125</v>
+        <v>2102</v>
       </c>
       <c r="C247" t="s">
         <v>1640</v>
@@ -17690,7 +17698,7 @@
         <v>1877</v>
       </c>
       <c r="B248" t="s">
-        <v>2126</v>
+        <v>2103</v>
       </c>
       <c r="C248" t="s">
         <v>1641</v>
@@ -17704,7 +17712,7 @@
         <v>1878</v>
       </c>
       <c r="B249" t="s">
-        <v>2127</v>
+        <v>2104</v>
       </c>
       <c r="C249" t="s">
         <v>1642</v>
@@ -17718,7 +17726,7 @@
         <v>1879</v>
       </c>
       <c r="B250" t="s">
-        <v>2128</v>
+        <v>2105</v>
       </c>
       <c r="C250" t="s">
         <v>1643</v>
@@ -17732,7 +17740,7 @@
         <v>301</v>
       </c>
       <c r="B251" t="s">
-        <v>2129</v>
+        <v>2106</v>
       </c>
       <c r="C251" t="s">
         <v>1644</v>

</xml_diff>